<commit_message>
start long stroke potential energy analysis
</commit_message>
<xml_diff>
--- a/pulley.xlsx
+++ b/pulley.xlsx
@@ -13,319 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
-  <si>
-    <t>Var1</t>
-  </si>
-  <si>
-    <t>Var2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Var1</t>
   </si>
@@ -381,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -395,63 +83,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -459,58 +95,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,15 +108,15 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="14.37890625" customWidth="true"/>
+    <col min="2" max="2" width="14.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
added force balance calculations
</commit_message>
<xml_diff>
--- a/pulley.xlsx
+++ b/pulley.xlsx
@@ -13,7 +13,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
+  <si>
+    <t>Var1</t>
+  </si>
+  <si>
+    <t>Var2</t>
+  </si>
   <si>
     <t>Var1</t>
   </si>
@@ -69,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -83,11 +161,24 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -95,6 +186,19 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,10 +217,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">

</xml_diff>